<commit_message>
Ultimas modificaciones a EFs de Telcodata
Cambios en inventarios y costo de ventas
</commit_message>
<xml_diff>
--- a/FASE II - Ejecucion/7000 Pruebas de Resultados/7100 Ingresos/7111 Facturas emitidas 2020/TELCODATA - DETALLE FACTURA VENTAS OCT 2020.xlsx
+++ b/FASE II - Ejecucion/7000 Pruebas de Resultados/7100 Ingresos/7111 Facturas emitidas 2020/TELCODATA - DETALLE FACTURA VENTAS OCT 2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Almeida\Documents\GitHub\TELCODATA\FASE II - Ejecucion\7000 Pruebas de Resultados\7100 Ingresos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Almeida\Documents\GitHub\TELCODATA\FASE II - Ejecucion\7000 Pruebas de Resultados\7100 Ingresos\7111 Facturas emitidas 2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22704C4-F744-4765-B6E3-DED60648FCDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC86977-E966-4113-8CD1-8A9296E3B860}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Fecha Fact.</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>290 DRY BATTERY  HR-1280</t>
+  </si>
+  <si>
+    <t>COSTO DE VENTAS</t>
+  </si>
+  <si>
+    <t>MARGEN $</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -82,7 +91,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,16 +113,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,11 +143,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -136,9 +174,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -416,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +480,7 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +499,17 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43882</v>
       </c>
@@ -470,8 +528,16 @@
       <c r="F2" s="5">
         <v>69171.199999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="13">
+        <f>+D2-H2</f>
+        <v>61760</v>
+      </c>
+      <c r="J2" s="14" t="e">
+        <f>+I2/H2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43906</v>
       </c>
@@ -490,8 +556,16 @@
       <c r="F3" s="5">
         <v>86016</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="13">
+        <f t="shared" ref="I3:I9" si="0">+D3-H3</f>
+        <v>76800</v>
+      </c>
+      <c r="J3" s="14" t="e">
+        <f t="shared" ref="J3:J9" si="1">+I3/H3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44005</v>
       </c>
@@ -510,8 +584,16 @@
       <c r="F4" s="6">
         <v>52640</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="13">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="J4" s="14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44006</v>
       </c>
@@ -530,8 +612,16 @@
       <c r="F5" s="6">
         <v>18480</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="13">
+        <f t="shared" si="0"/>
+        <v>16500</v>
+      </c>
+      <c r="J5" s="14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44014</v>
       </c>
@@ -550,8 +640,16 @@
       <c r="F6" s="6">
         <v>52640</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="13">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="J6" s="14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44052</v>
       </c>
@@ -570,8 +668,16 @@
       <c r="F7" s="6">
         <v>26320</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="13">
+        <f t="shared" si="0"/>
+        <v>23500</v>
+      </c>
+      <c r="J7" s="14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44064</v>
       </c>
@@ -590,8 +696,16 @@
       <c r="F8" s="6">
         <v>68040</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="13">
+        <f t="shared" si="0"/>
+        <v>60750</v>
+      </c>
+      <c r="J8" s="14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>44065</v>
       </c>
@@ -610,8 +724,27 @@
       <c r="F9" s="6">
         <v>50344</v>
       </c>
+      <c r="I9" s="13">
+        <f t="shared" si="0"/>
+        <v>44950</v>
+      </c>
+      <c r="J9" s="14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="10">
+        <f>SUM(D2:D9)</f>
+        <v>378260</v>
+      </c>
+      <c r="H10" s="15">
+        <f>SUM(H2:H9)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>